<commit_message>
update ids of parking spots
</commit_message>
<xml_diff>
--- a/sources/parking-spots/ulm_sensors.xlsx
+++ b/sources/parking-spots/ulm_sensors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\my-system-c\ipl\data\xlsx\ulm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BBD5E6-E59C-419B-81AE-75B2B1ECBD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C864E20-4B5C-4127-B2FB-B08C034E2DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2FAF8A27-CC6F-4E11-A521-588849C98525}"/>
   </bookViews>
@@ -128,273 +128,9 @@
     <t xml:space="preserve">Parkhaus Salzstadel                                                                                                                                                                                                                                     </t>
   </si>
   <si>
-    <t>pbg-s-eladen-1-01_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-02_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-03_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-04_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-05_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-06_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-07_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-08_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-09_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-10_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-11_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-12_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-13_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-14_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-15_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-16_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-17_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-18_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-19_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
-    <t>pbg-s-eladen-1-20_C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
     <t>Ladesäule</t>
   </si>
   <si>
-    <t>pbg-f-eladen-0-01_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-02_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-03_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-04_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-05_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-06_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-07_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-08_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-09_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-10_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-11_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-12_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-13_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-14_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-15_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-16_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-17_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-18_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-19_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-f-eladen-0-20_132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
-    <t>pbg-c01-19296d_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c02-1921b0_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c03-192985_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c04-192995_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c05-1921cd_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c06-1921dd_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c07-192968_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c08-1921da_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c09-192980_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c10-1921bc_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c11-192996_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c12-19298a_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c13-1921bb_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c14-1921d4_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c15-192987_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-c16-19297d_057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
-    <t>pbg-r01-192851_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r02-19284f_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r03-192839_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r04-192835_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r05-192837_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r06-192838_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r07-192832_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r08-192834_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r09-192833_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r10-192836_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r11-192830_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r12-192831_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r13-19283c_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r14-19283d_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r15-19283b_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r16-19283a_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r17-192827_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r18-19283e_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r19-19283f_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r20-192840_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r21-19282f_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r22-19282e_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r23-192841_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r24-19282c_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r25-192842_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r26-19282b_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r27-19282d_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r28-19282a_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r29-192829_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r30-192825_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r31-192826_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
-    <t>pbg-r32-192828_6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
     <t>Familie</t>
   </si>
   <si>
@@ -404,175 +140,439 @@
     <t>Nicht zugeordnet (kann ignoriert werden)</t>
   </si>
   <si>
-    <t>pbg-b-elade-o-1-006_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-007_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-008_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-009_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-010_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-011_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-012_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-013_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-014_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-015_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-016_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-017_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-018_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-019_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-020_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-o-1-021_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-054_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-055_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-056_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-057_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-058_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-059_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-060_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-061_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-062_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-063_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-064_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-065_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-066_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-067_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-068_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-elade-w-1-069_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-o-1-001_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-o-1-002_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-o-2-001_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-o-2-002_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-o-3-001_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-o-3-002_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-o-4-001_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-o-4-002_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-w-1-003_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-w-1-004_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-w-2-003_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-w-2-004_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-w-3-003_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-w-3-004_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-w-4-003_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-familie-w-4-004_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-handicap-o-1-001_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-handicap-o-2-001_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-handicap-o-3-001_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-handicap-o-4-001_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-handicap-w-2-002_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-handicap-w-3-002_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
-    <t>pbg-b-handicap-w-4-002_6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
-  </si>
-  <si>
     <t>Widmung</t>
   </si>
   <si>
     <t>Geometry</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-01</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-02</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-03</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-04</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-05</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-06</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-07</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-08</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-09</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-10</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-11</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-12</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-13</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-14</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-15</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-16</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-17</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-18</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-19</t>
+  </si>
+  <si>
+    <t>pbg-s-eladen-1-20</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-01</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-02</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-03</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-04</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-05</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-06</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-07</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-08</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-09</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-10</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-11</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-12</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-13</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-14</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-15</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-16</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-17</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-18</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-19</t>
+  </si>
+  <si>
+    <t>pbg-f-eladen-0-20</t>
+  </si>
+  <si>
+    <t>pbg-c01-19296d</t>
+  </si>
+  <si>
+    <t>pbg-c02-1921b0</t>
+  </si>
+  <si>
+    <t>pbg-c03-192985</t>
+  </si>
+  <si>
+    <t>pbg-c04-192995</t>
+  </si>
+  <si>
+    <t>pbg-c05-1921cd</t>
+  </si>
+  <si>
+    <t>pbg-c06-1921dd</t>
+  </si>
+  <si>
+    <t>pbg-c07-192968</t>
+  </si>
+  <si>
+    <t>pbg-c08-1921da</t>
+  </si>
+  <si>
+    <t>pbg-c09-192980</t>
+  </si>
+  <si>
+    <t>pbg-c10-1921bc</t>
+  </si>
+  <si>
+    <t>pbg-c11-192996</t>
+  </si>
+  <si>
+    <t>pbg-c12-19298a</t>
+  </si>
+  <si>
+    <t>pbg-c13-1921bb</t>
+  </si>
+  <si>
+    <t>pbg-c14-1921d4</t>
+  </si>
+  <si>
+    <t>pbg-c15-192987</t>
+  </si>
+  <si>
+    <t>pbg-c16-19297d</t>
+  </si>
+  <si>
+    <t>pbg-r01-192851</t>
+  </si>
+  <si>
+    <t>pbg-r02-19284f</t>
+  </si>
+  <si>
+    <t>pbg-r03-192839</t>
+  </si>
+  <si>
+    <t>pbg-r04-192835</t>
+  </si>
+  <si>
+    <t>pbg-r05-192837</t>
+  </si>
+  <si>
+    <t>pbg-r06-192838</t>
+  </si>
+  <si>
+    <t>pbg-r07-192832</t>
+  </si>
+  <si>
+    <t>pbg-r08-192834</t>
+  </si>
+  <si>
+    <t>pbg-r09-192833</t>
+  </si>
+  <si>
+    <t>pbg-r10-192836</t>
+  </si>
+  <si>
+    <t>pbg-r11-192830</t>
+  </si>
+  <si>
+    <t>pbg-r12-192831</t>
+  </si>
+  <si>
+    <t>pbg-r13-19283c</t>
+  </si>
+  <si>
+    <t>pbg-r14-19283d</t>
+  </si>
+  <si>
+    <t>pbg-r15-19283b</t>
+  </si>
+  <si>
+    <t>pbg-r16-19283a</t>
+  </si>
+  <si>
+    <t>pbg-r17-192827</t>
+  </si>
+  <si>
+    <t>pbg-r18-19283e</t>
+  </si>
+  <si>
+    <t>pbg-r19-19283f</t>
+  </si>
+  <si>
+    <t>pbg-r20-192840</t>
+  </si>
+  <si>
+    <t>pbg-r21-19282f</t>
+  </si>
+  <si>
+    <t>pbg-r22-19282e</t>
+  </si>
+  <si>
+    <t>pbg-r23-192841</t>
+  </si>
+  <si>
+    <t>pbg-r24-19282c</t>
+  </si>
+  <si>
+    <t>pbg-r25-192842</t>
+  </si>
+  <si>
+    <t>pbg-r26-19282b</t>
+  </si>
+  <si>
+    <t>pbg-r27-19282d</t>
+  </si>
+  <si>
+    <t>pbg-r28-19282a</t>
+  </si>
+  <si>
+    <t>pbg-r29-192829</t>
+  </si>
+  <si>
+    <t>pbg-r30-192825</t>
+  </si>
+  <si>
+    <t>pbg-r31-192826</t>
+  </si>
+  <si>
+    <t>pbg-r32-192828</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-006</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-007</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-008</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-009</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-010</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-011</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-012</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-013</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-014</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-015</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-016</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-017</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-018</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-019</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-020</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-o-1-021</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-054</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-055</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-056</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-057</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-058</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-059</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-060</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-061</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-062</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-063</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-064</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-065</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-066</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-067</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-068</t>
+  </si>
+  <si>
+    <t>pbg-b-elade-w-1-069</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-o-1-001</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-o-1-002</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-o-2-001</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-o-2-002</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-o-3-001</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-o-3-002</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-o-4-001</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-o-4-002</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-w-1-003</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-w-1-004</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-w-2-003</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-w-2-004</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-w-3-003</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-w-3-004</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-w-4-003</t>
+  </si>
+  <si>
+    <t>pbg-b-familie-w-4-004</t>
+  </si>
+  <si>
+    <t>pbg-b-handicap-o-1-001</t>
+  </si>
+  <si>
+    <t>pbg-b-handicap-o-2-001</t>
+  </si>
+  <si>
+    <t>pbg-b-handicap-o-3-001</t>
+  </si>
+  <si>
+    <t>pbg-b-handicap-o-4-001</t>
+  </si>
+  <si>
+    <t>pbg-b-handicap-w-2-002</t>
+  </si>
+  <si>
+    <t>pbg-b-handicap-w-3-002</t>
+  </si>
+  <si>
+    <t>pbg-b-handicap-w-4-002</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54411EF9-4ECD-406D-85AB-8CEFA9039220}">
   <dimension ref="A1:AD144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1046,7 +1046,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1055,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>169</v>
+        <v>26</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>4</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -1106,7 +1106,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E2" s="3">
         <v>48.4011345561022</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -1130,7 +1130,7 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3">
         <v>48.4011345561022</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -1154,7 +1154,7 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3">
         <v>48.4011345561022</v>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -1178,7 +1178,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3">
         <v>48.4011345561022</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -1202,7 +1202,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3">
         <v>48.4011345561022</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -1226,7 +1226,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3">
         <v>48.4011345561022</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -1250,7 +1250,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3">
         <v>48.4011345561022</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -1274,7 +1274,7 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3">
         <v>48.4011345561022</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -1298,7 +1298,7 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3">
         <v>48.4011345561022</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
@@ -1322,7 +1322,7 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3">
         <v>48.4011345561022</v>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
@@ -1346,7 +1346,7 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E12" s="3">
         <v>48.4011345561022</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -1370,7 +1370,7 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E13" s="3">
         <v>48.4011345561022</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
@@ -1394,7 +1394,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E14" s="3">
         <v>48.4011345561022</v>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
@@ -1418,7 +1418,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3">
         <v>48.4011345561022</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
@@ -1442,7 +1442,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E16" s="3">
         <v>48.4011345561022</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
@@ -1466,7 +1466,7 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E17" s="3">
         <v>48.4011345561022</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
@@ -1490,7 +1490,7 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E18" s="3">
         <v>48.4011345561022</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1514,7 +1514,7 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E19" s="3">
         <v>48.4011345561022</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -1538,7 +1538,7 @@
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3">
         <v>48.4011345561022</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -1562,7 +1562,7 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E21" s="3">
         <v>48.4011345561022</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
@@ -1586,7 +1586,7 @@
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E22" s="3">
         <v>48.396582769184</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
         <v>15</v>
@@ -1610,7 +1610,7 @@
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E23" s="3">
         <v>48.396582769184</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
@@ -1634,7 +1634,7 @@
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E24" s="3">
         <v>48.396582769184</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
@@ -1658,7 +1658,7 @@
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E25" s="3">
         <v>48.396582769184</v>
@@ -1673,7 +1673,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
@@ -1682,7 +1682,7 @@
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E26" s="3">
         <v>48.396582769184</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
@@ -1706,7 +1706,7 @@
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E27" s="3">
         <v>48.396582769184</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
@@ -1730,7 +1730,7 @@
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E28" s="3">
         <v>48.396582769184</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
@@ -1754,7 +1754,7 @@
         <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E29" s="3">
         <v>48.396582769184</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
@@ -1778,7 +1778,7 @@
         <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E30" s="3">
         <v>48.396582769184</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
@@ -1802,7 +1802,7 @@
         <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E31" s="3">
         <v>48.396582769184</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
         <v>15</v>
@@ -1826,7 +1826,7 @@
         <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E32" s="3">
         <v>48.396582769184</v>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
         <v>15</v>
@@ -1850,7 +1850,7 @@
         <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E33" s="3">
         <v>48.396582769184</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
         <v>15</v>
@@ -1874,7 +1874,7 @@
         <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E34" s="3">
         <v>48.396582769184</v>
@@ -1889,7 +1889,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
@@ -1898,7 +1898,7 @@
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E35" s="3">
         <v>48.396582769184</v>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
@@ -1922,7 +1922,7 @@
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E36" s="3">
         <v>48.396582769184</v>
@@ -1937,7 +1937,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
@@ -1946,7 +1946,7 @@
         <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E37" s="3">
         <v>48.396582769184</v>
@@ -1961,7 +1961,7 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
@@ -1970,7 +1970,7 @@
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E38" s="3">
         <v>48.396582769184</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
@@ -1994,7 +1994,7 @@
         <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E39" s="3">
         <v>48.396582769184</v>
@@ -2009,7 +2009,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
         <v>15</v>
@@ -2018,7 +2018,7 @@
         <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E40" s="3">
         <v>48.396582769184</v>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
@@ -2042,7 +2042,7 @@
         <v>14</v>
       </c>
       <c r="D41" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E41" s="3">
         <v>48.396582769184</v>
@@ -2057,7 +2057,7 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
@@ -2066,7 +2066,7 @@
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E42" s="3">
         <v>48.401631838230998</v>
@@ -2097,7 +2097,7 @@
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
         <v>16</v>
@@ -2106,7 +2106,7 @@
         <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E43" s="3">
         <v>48.401631838230998</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
         <v>16</v>
@@ -2146,7 +2146,7 @@
         <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E44" s="3">
         <v>48.401631838230998</v>
@@ -2177,7 +2177,7 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
         <v>16</v>
@@ -2186,7 +2186,7 @@
         <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E45" s="3">
         <v>48.401631838230998</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
         <v>16</v>
@@ -2226,7 +2226,7 @@
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E46" s="3">
         <v>48.401631838230998</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
         <v>16</v>
@@ -2266,7 +2266,7 @@
         <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E47" s="3">
         <v>48.401631838230998</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
         <v>16</v>
@@ -2306,7 +2306,7 @@
         <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E48" s="3">
         <v>48.401631838230998</v>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
@@ -2346,7 +2346,7 @@
         <v>14</v>
       </c>
       <c r="D49" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E49" s="3">
         <v>48.401631838230998</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
@@ -2386,7 +2386,7 @@
         <v>14</v>
       </c>
       <c r="D50" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E50" s="3">
         <v>48.401631838230998</v>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
         <v>16</v>
@@ -2426,7 +2426,7 @@
         <v>14</v>
       </c>
       <c r="D51" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E51" s="3">
         <v>48.401631838230998</v>
@@ -2457,7 +2457,7 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
         <v>16</v>
@@ -2466,7 +2466,7 @@
         <v>14</v>
       </c>
       <c r="D52" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E52" s="3">
         <v>48.401631838230998</v>
@@ -2497,7 +2497,7 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
         <v>16</v>
@@ -2506,7 +2506,7 @@
         <v>14</v>
       </c>
       <c r="D53" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E53" s="3">
         <v>48.401631838230998</v>
@@ -2537,7 +2537,7 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
         <v>16</v>
@@ -2546,7 +2546,7 @@
         <v>14</v>
       </c>
       <c r="D54" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E54" s="3">
         <v>48.401631838230998</v>
@@ -2577,7 +2577,7 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B55" t="s">
         <v>16</v>
@@ -2586,7 +2586,7 @@
         <v>14</v>
       </c>
       <c r="D55" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E55" s="3">
         <v>48.401631838230998</v>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B56" t="s">
         <v>16</v>
@@ -2626,7 +2626,7 @@
         <v>14</v>
       </c>
       <c r="D56" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E56" s="3">
         <v>48.401631838230998</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
         <v>16</v>
@@ -2666,7 +2666,7 @@
         <v>14</v>
       </c>
       <c r="D57" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E57" s="3">
         <v>48.401631838230998</v>
@@ -2697,7 +2697,7 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
@@ -2706,7 +2706,7 @@
         <v>14</v>
       </c>
       <c r="D58" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E58" s="3">
         <v>48.397248418725397</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
@@ -2730,7 +2730,7 @@
         <v>14</v>
       </c>
       <c r="D59" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E59" s="3">
         <v>48.397248418725397</v>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B60" t="s">
         <v>18</v>
@@ -2754,7 +2754,7 @@
         <v>14</v>
       </c>
       <c r="D60" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E60" s="3">
         <v>48.397248418725397</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
         <v>18</v>
@@ -2778,7 +2778,7 @@
         <v>14</v>
       </c>
       <c r="D61" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E61" s="3">
         <v>48.397248418725397</v>
@@ -2793,7 +2793,7 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B62" t="s">
         <v>18</v>
@@ -2802,7 +2802,7 @@
         <v>14</v>
       </c>
       <c r="D62" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E62" s="3">
         <v>48.397248418725397</v>
@@ -2817,7 +2817,7 @@
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
         <v>18</v>
@@ -2826,7 +2826,7 @@
         <v>14</v>
       </c>
       <c r="D63" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E63" s="3">
         <v>48.397248418725397</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
         <v>18</v>
@@ -2850,7 +2850,7 @@
         <v>14</v>
       </c>
       <c r="D64" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E64" s="3">
         <v>48.397248418725397</v>
@@ -2865,7 +2865,7 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B65" t="s">
         <v>18</v>
@@ -2874,7 +2874,7 @@
         <v>14</v>
       </c>
       <c r="D65" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E65" s="3">
         <v>48.397248418725397</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
         <v>18</v>
@@ -2898,7 +2898,7 @@
         <v>14</v>
       </c>
       <c r="D66" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E66" s="3">
         <v>48.397248418725397</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B67" t="s">
         <v>18</v>
@@ -2922,7 +2922,7 @@
         <v>14</v>
       </c>
       <c r="D67" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E67" s="3">
         <v>48.397248418725397</v>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B68" t="s">
         <v>18</v>
@@ -2946,7 +2946,7 @@
         <v>14</v>
       </c>
       <c r="D68" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E68" s="3">
         <v>48.397248418725397</v>
@@ -2961,7 +2961,7 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B69" t="s">
         <v>18</v>
@@ -2970,7 +2970,7 @@
         <v>14</v>
       </c>
       <c r="D69" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E69" s="3">
         <v>48.397248418725397</v>
@@ -2985,7 +2985,7 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A70" s="7" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B70" t="s">
         <v>18</v>
@@ -2994,7 +2994,7 @@
         <v>14</v>
       </c>
       <c r="D70" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E70" s="3">
         <v>48.397248418725397</v>
@@ -3009,7 +3009,7 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B71" t="s">
         <v>18</v>
@@ -3018,7 +3018,7 @@
         <v>14</v>
       </c>
       <c r="D71" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E71" s="3">
         <v>48.397248418725397</v>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B72" t="s">
         <v>18</v>
@@ -3042,7 +3042,7 @@
         <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E72" s="3">
         <v>48.397248418725397</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A73" s="7" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B73" t="s">
         <v>18</v>
@@ -3066,7 +3066,7 @@
         <v>14</v>
       </c>
       <c r="D73" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E73" s="3">
         <v>48.397248418725397</v>
@@ -3081,7 +3081,7 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B74" t="s">
         <v>18</v>
@@ -3090,7 +3090,7 @@
         <v>14</v>
       </c>
       <c r="D74" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E74" s="3">
         <v>48.397248418725397</v>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B75" t="s">
         <v>18</v>
@@ -3114,7 +3114,7 @@
         <v>14</v>
       </c>
       <c r="D75" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E75" s="3">
         <v>48.397248418725397</v>
@@ -3129,7 +3129,7 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A76" s="7" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B76" t="s">
         <v>18</v>
@@ -3138,7 +3138,7 @@
         <v>14</v>
       </c>
       <c r="D76" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E76" s="3">
         <v>48.397248418725397</v>
@@ -3153,7 +3153,7 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B77" t="s">
         <v>18</v>
@@ -3162,7 +3162,7 @@
         <v>14</v>
       </c>
       <c r="D77" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E77" s="3">
         <v>48.397248418725397</v>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A78" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B78" t="s">
         <v>18</v>
@@ -3186,7 +3186,7 @@
         <v>14</v>
       </c>
       <c r="D78" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E78" s="3">
         <v>48.397248418725397</v>
@@ -3201,7 +3201,7 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A79" s="7" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B79" t="s">
         <v>18</v>
@@ -3210,7 +3210,7 @@
         <v>14</v>
       </c>
       <c r="D79" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E79" s="3">
         <v>48.397248418725397</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A80" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B80" t="s">
         <v>18</v>
@@ -3234,7 +3234,7 @@
         <v>14</v>
       </c>
       <c r="D80" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E80" s="3">
         <v>48.397248418725397</v>
@@ -3249,7 +3249,7 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B81" t="s">
         <v>18</v>
@@ -3258,7 +3258,7 @@
         <v>14</v>
       </c>
       <c r="D81" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E81" s="3">
         <v>48.397248418725397</v>
@@ -3273,7 +3273,7 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A82" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B82" t="s">
         <v>18</v>
@@ -3282,7 +3282,7 @@
         <v>14</v>
       </c>
       <c r="D82" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E82" s="3">
         <v>48.397248418725397</v>
@@ -3297,7 +3297,7 @@
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B83" t="s">
         <v>18</v>
@@ -3306,7 +3306,7 @@
         <v>14</v>
       </c>
       <c r="D83" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E83" s="3">
         <v>48.397248418725397</v>
@@ -3321,7 +3321,7 @@
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A84" s="7" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B84" t="s">
         <v>18</v>
@@ -3330,7 +3330,7 @@
         <v>14</v>
       </c>
       <c r="D84" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E84" s="3">
         <v>48.397248418725397</v>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A85" s="7" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B85" t="s">
         <v>18</v>
@@ -3354,7 +3354,7 @@
         <v>14</v>
       </c>
       <c r="D85" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E85" s="3">
         <v>48.397248418725397</v>
@@ -3369,7 +3369,7 @@
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A86" s="7" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B86" t="s">
         <v>18</v>
@@ -3378,7 +3378,7 @@
         <v>14</v>
       </c>
       <c r="D86" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E86" s="3">
         <v>48.397248418725397</v>
@@ -3393,7 +3393,7 @@
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A87" s="7" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B87" t="s">
         <v>18</v>
@@ -3402,7 +3402,7 @@
         <v>14</v>
       </c>
       <c r="D87" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E87" s="3">
         <v>48.397248418725397</v>
@@ -3417,7 +3417,7 @@
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A88" s="7" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B88" t="s">
         <v>18</v>
@@ -3426,7 +3426,7 @@
         <v>14</v>
       </c>
       <c r="D88" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="E88" s="3">
         <v>48.397248418725397</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B89" t="s">
         <v>18</v>
@@ -3450,7 +3450,7 @@
         <v>14</v>
       </c>
       <c r="D89" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="E89" s="3">
         <v>48.397248418725397</v>
@@ -3465,7 +3465,7 @@
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A90" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B90" t="s">
         <v>19</v>
@@ -3474,7 +3474,7 @@
         <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E90" s="3">
         <v>48.398229802932498</v>
@@ -3495,7 +3495,7 @@
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B91" t="s">
         <v>19</v>
@@ -3504,7 +3504,7 @@
         <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E91" s="3">
         <v>48.398229802932498</v>
@@ -3525,7 +3525,7 @@
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A92" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B92" t="s">
         <v>19</v>
@@ -3534,7 +3534,7 @@
         <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E92" s="3">
         <v>48.398229802932498</v>
@@ -3555,7 +3555,7 @@
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A93" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B93" t="s">
         <v>19</v>
@@ -3564,7 +3564,7 @@
         <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E93" s="3">
         <v>48.398229802932498</v>
@@ -3585,7 +3585,7 @@
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A94" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B94" t="s">
         <v>19</v>
@@ -3594,7 +3594,7 @@
         <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E94" s="3">
         <v>48.398229802932498</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B95" t="s">
         <v>19</v>
@@ -3624,7 +3624,7 @@
         <v>14</v>
       </c>
       <c r="D95" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E95" s="3">
         <v>48.398229802932498</v>
@@ -3645,7 +3645,7 @@
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B96" t="s">
         <v>19</v>
@@ -3654,7 +3654,7 @@
         <v>14</v>
       </c>
       <c r="D96" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E96" s="3">
         <v>48.398229802932498</v>
@@ -3675,7 +3675,7 @@
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A97" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B97" t="s">
         <v>19</v>
@@ -3684,7 +3684,7 @@
         <v>14</v>
       </c>
       <c r="D97" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E97" s="3">
         <v>48.398229802932498</v>
@@ -3705,7 +3705,7 @@
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B98" t="s">
         <v>19</v>
@@ -3714,7 +3714,7 @@
         <v>14</v>
       </c>
       <c r="D98" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E98" s="3">
         <v>48.398229802932498</v>
@@ -3735,7 +3735,7 @@
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A99" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B99" t="s">
         <v>19</v>
@@ -3744,7 +3744,7 @@
         <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E99" s="3">
         <v>48.398229802932498</v>
@@ -3765,7 +3765,7 @@
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A100" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B100" t="s">
         <v>19</v>
@@ -3774,7 +3774,7 @@
         <v>14</v>
       </c>
       <c r="D100" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E100" s="3">
         <v>48.398229802932498</v>
@@ -3795,7 +3795,7 @@
     </row>
     <row r="101" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A101" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B101" t="s">
         <v>19</v>
@@ -3804,7 +3804,7 @@
         <v>14</v>
       </c>
       <c r="D101" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E101" s="3">
         <v>48.398229802932498</v>
@@ -3825,7 +3825,7 @@
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A102" s="7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B102" t="s">
         <v>19</v>
@@ -3834,7 +3834,7 @@
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E102" s="3">
         <v>48.398229802932498</v>
@@ -3855,7 +3855,7 @@
     </row>
     <row r="103" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A103" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B103" t="s">
         <v>19</v>
@@ -3864,7 +3864,7 @@
         <v>14</v>
       </c>
       <c r="D103" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E103" s="3">
         <v>48.398229802932498</v>
@@ -3885,7 +3885,7 @@
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A104" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B104" t="s">
         <v>19</v>
@@ -3894,7 +3894,7 @@
         <v>14</v>
       </c>
       <c r="D104" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E104" s="3">
         <v>48.398229802932498</v>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="105" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A105" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B105" t="s">
         <v>19</v>
@@ -3924,7 +3924,7 @@
         <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E105" s="3">
         <v>48.398229802932498</v>
@@ -3945,7 +3945,7 @@
     </row>
     <row r="106" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A106" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B106" t="s">
         <v>19</v>
@@ -3954,7 +3954,7 @@
         <v>14</v>
       </c>
       <c r="D106" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E106" s="3">
         <v>48.398229802932498</v>
@@ -3975,7 +3975,7 @@
     </row>
     <row r="107" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A107" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B107" t="s">
         <v>19</v>
@@ -3984,7 +3984,7 @@
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E107" s="3">
         <v>48.398229802932498</v>
@@ -4005,7 +4005,7 @@
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A108" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B108" t="s">
         <v>19</v>
@@ -4014,7 +4014,7 @@
         <v>14</v>
       </c>
       <c r="D108" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E108" s="3">
         <v>48.398229802932498</v>
@@ -4035,7 +4035,7 @@
     </row>
     <row r="109" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A109" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B109" t="s">
         <v>19</v>
@@ -4044,7 +4044,7 @@
         <v>14</v>
       </c>
       <c r="D109" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E109" s="3">
         <v>48.398229802932498</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="110" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A110" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B110" t="s">
         <v>19</v>
@@ -4074,7 +4074,7 @@
         <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E110" s="3">
         <v>48.398229802932498</v>
@@ -4095,7 +4095,7 @@
     </row>
     <row r="111" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A111" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B111" t="s">
         <v>19</v>
@@ -4104,7 +4104,7 @@
         <v>14</v>
       </c>
       <c r="D111" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E111" s="3">
         <v>48.398229802932498</v>
@@ -4125,7 +4125,7 @@
     </row>
     <row r="112" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A112" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B112" t="s">
         <v>19</v>
@@ -4134,7 +4134,7 @@
         <v>14</v>
       </c>
       <c r="D112" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E112" s="3">
         <v>48.398229802932498</v>
@@ -4155,7 +4155,7 @@
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A113" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B113" t="s">
         <v>19</v>
@@ -4164,7 +4164,7 @@
         <v>14</v>
       </c>
       <c r="D113" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E113" s="3">
         <v>48.398229802932498</v>
@@ -4185,7 +4185,7 @@
     </row>
     <row r="114" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A114" s="7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B114" t="s">
         <v>19</v>
@@ -4194,7 +4194,7 @@
         <v>14</v>
       </c>
       <c r="D114" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E114" s="3">
         <v>48.398229802932498</v>
@@ -4215,7 +4215,7 @@
     </row>
     <row r="115" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A115" s="7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B115" t="s">
         <v>19</v>
@@ -4224,7 +4224,7 @@
         <v>14</v>
       </c>
       <c r="D115" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E115" s="3">
         <v>48.398229802932498</v>
@@ -4245,7 +4245,7 @@
     </row>
     <row r="116" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A116" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B116" t="s">
         <v>19</v>
@@ -4254,7 +4254,7 @@
         <v>14</v>
       </c>
       <c r="D116" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E116" s="3">
         <v>48.398229802932498</v>
@@ -4275,7 +4275,7 @@
     </row>
     <row r="117" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A117" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B117" t="s">
         <v>19</v>
@@ -4284,7 +4284,7 @@
         <v>14</v>
       </c>
       <c r="D117" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E117" s="3">
         <v>48.398229802932498</v>
@@ -4305,7 +4305,7 @@
     </row>
     <row r="118" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A118" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B118" t="s">
         <v>19</v>
@@ -4314,7 +4314,7 @@
         <v>14</v>
       </c>
       <c r="D118" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E118" s="3">
         <v>48.398229802932498</v>
@@ -4335,7 +4335,7 @@
     </row>
     <row r="119" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A119" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B119" t="s">
         <v>19</v>
@@ -4344,7 +4344,7 @@
         <v>14</v>
       </c>
       <c r="D119" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E119" s="3">
         <v>48.398229802932498</v>
@@ -4365,7 +4365,7 @@
     </row>
     <row r="120" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A120" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B120" t="s">
         <v>19</v>
@@ -4374,7 +4374,7 @@
         <v>14</v>
       </c>
       <c r="D120" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E120" s="3">
         <v>48.398229802932498</v>
@@ -4395,7 +4395,7 @@
     </row>
     <row r="121" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A121" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B121" t="s">
         <v>19</v>
@@ -4404,7 +4404,7 @@
         <v>14</v>
       </c>
       <c r="D121" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E121" s="3">
         <v>48.398229802932498</v>
@@ -4425,7 +4425,7 @@
     </row>
     <row r="122" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A122" s="7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B122" t="s">
         <v>19</v>
@@ -4434,7 +4434,7 @@
         <v>14</v>
       </c>
       <c r="D122" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E122" s="3">
         <v>48.398229802932498</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="123" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A123" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B123" t="s">
         <v>19</v>
@@ -4464,7 +4464,7 @@
         <v>14</v>
       </c>
       <c r="D123" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E123" s="3">
         <v>48.398229802932498</v>
@@ -4485,7 +4485,7 @@
     </row>
     <row r="124" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A124" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B124" t="s">
         <v>19</v>
@@ -4494,7 +4494,7 @@
         <v>14</v>
       </c>
       <c r="D124" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E124" s="3">
         <v>48.398229802932498</v>
@@ -4515,7 +4515,7 @@
     </row>
     <row r="125" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A125" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B125" t="s">
         <v>19</v>
@@ -4524,7 +4524,7 @@
         <v>14</v>
       </c>
       <c r="D125" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E125" s="3">
         <v>48.398229802932498</v>
@@ -4545,7 +4545,7 @@
     </row>
     <row r="126" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A126" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B126" t="s">
         <v>19</v>
@@ -4554,7 +4554,7 @@
         <v>14</v>
       </c>
       <c r="D126" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E126" s="3">
         <v>48.398229802932498</v>
@@ -4575,7 +4575,7 @@
     </row>
     <row r="127" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A127" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B127" t="s">
         <v>19</v>
@@ -4584,7 +4584,7 @@
         <v>14</v>
       </c>
       <c r="D127" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E127" s="3">
         <v>48.398229802932498</v>
@@ -4605,7 +4605,7 @@
     </row>
     <row r="128" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A128" s="7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B128" t="s">
         <v>19</v>
@@ -4614,7 +4614,7 @@
         <v>14</v>
       </c>
       <c r="D128" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E128" s="3">
         <v>48.398229802932498</v>
@@ -4635,7 +4635,7 @@
     </row>
     <row r="129" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A129" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B129" t="s">
         <v>19</v>
@@ -4644,7 +4644,7 @@
         <v>14</v>
       </c>
       <c r="D129" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E129" s="3">
         <v>48.398229802932498</v>
@@ -4665,7 +4665,7 @@
     </row>
     <row r="130" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A130" s="7" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B130" t="s">
         <v>19</v>
@@ -4674,7 +4674,7 @@
         <v>14</v>
       </c>
       <c r="D130" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E130" s="3">
         <v>48.398229802932498</v>
@@ -4695,7 +4695,7 @@
     </row>
     <row r="131" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A131" s="7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B131" t="s">
         <v>19</v>
@@ -4704,7 +4704,7 @@
         <v>14</v>
       </c>
       <c r="D131" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E131" s="3">
         <v>48.398229802932498</v>
@@ -4725,7 +4725,7 @@
     </row>
     <row r="132" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A132" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B132" t="s">
         <v>19</v>
@@ -4734,7 +4734,7 @@
         <v>14</v>
       </c>
       <c r="D132" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E132" s="3">
         <v>48.398229802932498</v>
@@ -4755,7 +4755,7 @@
     </row>
     <row r="133" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A133" s="7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B133" t="s">
         <v>19</v>
@@ -4764,7 +4764,7 @@
         <v>14</v>
       </c>
       <c r="D133" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E133" s="3">
         <v>48.398229802932498</v>
@@ -4785,7 +4785,7 @@
     </row>
     <row r="134" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A134" s="7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B134" t="s">
         <v>19</v>
@@ -4794,7 +4794,7 @@
         <v>14</v>
       </c>
       <c r="D134" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E134" s="3">
         <v>48.398229802932498</v>
@@ -4815,7 +4815,7 @@
     </row>
     <row r="135" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A135" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B135" t="s">
         <v>19</v>
@@ -4824,7 +4824,7 @@
         <v>14</v>
       </c>
       <c r="D135" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E135" s="3">
         <v>48.398229802932498</v>
@@ -4845,7 +4845,7 @@
     </row>
     <row r="136" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A136" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B136" t="s">
         <v>19</v>
@@ -4854,7 +4854,7 @@
         <v>14</v>
       </c>
       <c r="D136" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E136" s="3">
         <v>48.398229802932498</v>
@@ -4875,7 +4875,7 @@
     </row>
     <row r="137" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A137" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B137" t="s">
         <v>19</v>
@@ -4884,7 +4884,7 @@
         <v>14</v>
       </c>
       <c r="D137" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E137" s="3">
         <v>48.398229802932498</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="138" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A138" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B138" t="s">
         <v>19</v>
@@ -4914,7 +4914,7 @@
         <v>14</v>
       </c>
       <c r="D138" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E138" s="3">
         <v>48.398229802932498</v>
@@ -4935,7 +4935,7 @@
     </row>
     <row r="139" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A139" s="7" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B139" t="s">
         <v>19</v>
@@ -4944,7 +4944,7 @@
         <v>14</v>
       </c>
       <c r="D139" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E139" s="3">
         <v>48.398229802932498</v>
@@ -4965,7 +4965,7 @@
     </row>
     <row r="140" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A140" s="7" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B140" t="s">
         <v>19</v>
@@ -4974,7 +4974,7 @@
         <v>14</v>
       </c>
       <c r="D140" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E140" s="3">
         <v>48.398229802932498</v>
@@ -4995,7 +4995,7 @@
     </row>
     <row r="141" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A141" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B141" t="s">
         <v>19</v>
@@ -5004,7 +5004,7 @@
         <v>14</v>
       </c>
       <c r="D141" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E141" s="3">
         <v>48.398229802932498</v>
@@ -5025,7 +5025,7 @@
     </row>
     <row r="142" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A142" s="7" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B142" t="s">
         <v>19</v>
@@ -5034,7 +5034,7 @@
         <v>14</v>
       </c>
       <c r="D142" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E142" s="3">
         <v>48.398229802932498</v>
@@ -5055,7 +5055,7 @@
     </row>
     <row r="143" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A143" s="7" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B143" t="s">
         <v>19</v>
@@ -5064,7 +5064,7 @@
         <v>14</v>
       </c>
       <c r="D143" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E143" s="3">
         <v>48.398229802932498</v>
@@ -5085,7 +5085,7 @@
     </row>
     <row r="144" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A144" s="7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B144" t="s">
         <v>19</v>
@@ -5094,7 +5094,7 @@
         <v>14</v>
       </c>
       <c r="D144" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="E144" s="3">
         <v>48.398229802932498</v>

</xml_diff>

<commit_message>
Fix attribute type as optional in parking-spot
</commit_message>
<xml_diff>
--- a/sources/parking-spots/ulm_sensors.xlsx
+++ b/sources/parking-spots/ulm_sensors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\my-system-c\ipl\data\xlsx\ulm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC995CFE-D579-4373-81E6-F4C26CF2213D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C1FDA4-4AD8-4584-B3C6-0FFFFE4B8CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2FAF8A27-CC6F-4E11-A521-588849C98525}"/>
   </bookViews>
@@ -1029,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54411EF9-4ECD-406D-85AB-8CEFA9039220}">
   <dimension ref="A1:AE144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>